<commit_message>
reg data preparation - step 3
</commit_message>
<xml_diff>
--- a/output/determinants/variables_structure.xlsx
+++ b/output/determinants/variables_structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Main\DOCUMENTOS\3. MACHINE LEARNING\PYTHON_PROYECTS\LPC_Finance\output\determinants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F0C9F-B201-478D-96C3-F112D23A9FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072E1A63-C274-48F2-A4C8-7EB96FC4AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -96,9 +96,6 @@
     <t>company size</t>
   </si>
   <si>
-    <t>VOLUME_CV</t>
-  </si>
-  <si>
     <t>PRICE_TO_BOOK</t>
   </si>
   <si>
@@ -241,13 +238,43 @@
   </si>
   <si>
     <t>Return std or Price std</t>
+  </si>
+  <si>
+    <t>Last, mean, rmean, other</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>Last, mean, cv, rmean, corr, beta</t>
+  </si>
+  <si>
+    <t>Last, mean, rmean</t>
+  </si>
+  <si>
+    <t>Histo mean, streak proba, max streak</t>
+  </si>
+  <si>
+    <t>9d, 14d , 30d, adx mean, trend days, trend proba</t>
+  </si>
+  <si>
+    <t>mean disp, last dips</t>
+  </si>
+  <si>
+    <t>mean_number, last_number</t>
+  </si>
+  <si>
+    <t>inf, mv, mean, last, rmean</t>
+  </si>
+  <si>
+    <t>mean, last, rmean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,11 +290,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,13 +355,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +642,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -608,33 +651,33 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -655,13 +698,13 @@
         <v>1.5</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>59</v>
+      <c r="I2" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -681,18 +724,18 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -707,18 +750,18 @@
         <v>1.5</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -733,13 +776,13 @@
         <v>1.5</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -759,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -779,11 +822,11 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -796,12 +839,15 @@
         <v>19</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>20</v>
+      <c r="A9" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -813,55 +859,64 @@
         <v>19</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
       <c r="E11">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -869,7 +924,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -878,38 +933,41 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -917,61 +975,73 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>33</v>
+      <c r="A16" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -980,70 +1050,73 @@
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="F19" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
       <c r="E20">
         <v>1.5</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
         <v>41</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
       <c r="E21">
         <v>1.5</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
       <c r="E22">
         <v>1.5</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1068,35 +1141,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1115,12 +1188,12 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
determinant data preparation done
</commit_message>
<xml_diff>
--- a/output/determinants/variables_structure.xlsx
+++ b/output/determinants/variables_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Main\DOCUMENTOS\3. MACHINE LEARNING\PYTHON_PROYECTS\LPC_Finance\output\determinants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072E1A63-C274-48F2-A4C8-7EB96FC4AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107471B2-141A-4BB1-B83E-C2E469327759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="540" windowWidth="20325" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REGVARS" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -114,9 +114,6 @@
     <t>HURST_EXPONENT</t>
   </si>
   <si>
-    <t>BREAKS_NUMBER</t>
-  </si>
-  <si>
     <t>tendency change</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Norm o no norm</t>
-  </si>
-  <si>
     <t>QUESTIONS</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>SAVED</t>
   </si>
   <si>
-    <t>Spread return?</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -237,37 +228,403 @@
     <t>MEAN_ROLLING_STD_LT</t>
   </si>
   <si>
-    <t>Return std or Price std</t>
-  </si>
-  <si>
-    <t>Last, mean, rmean, other</t>
-  </si>
-  <si>
     <t>VOLUME</t>
   </si>
   <si>
-    <t>Last, mean, cv, rmean, corr, beta</t>
-  </si>
-  <si>
-    <t>Last, mean, rmean</t>
-  </si>
-  <si>
     <t>Histo mean, streak proba, max streak</t>
   </si>
   <si>
-    <t>9d, 14d , 30d, adx mean, trend days, trend proba</t>
-  </si>
-  <si>
-    <t>mean disp, last dips</t>
-  </si>
-  <si>
-    <t>mean_number, last_number</t>
-  </si>
-  <si>
-    <t>inf, mv, mean, last, rmean</t>
-  </si>
-  <si>
-    <t>mean, last, rmean</t>
+    <t>INDUSTRY DUMMIES</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>cualquiera, sin mv</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">gmean, rmean, dfrw, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>days</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>proba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mr</t>
+    </r>
+  </si>
+  <si>
+    <t>BREAKS_NUMBER_CUSUM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9d, 14d , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, adx mean,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> trend days, trend proba</t>
+    </r>
+  </si>
+  <si>
+    <t>no norm</t>
+  </si>
+  <si>
+    <t>close return vs spread "price"</t>
+  </si>
+  <si>
+    <t>close return vs sp500 close return</t>
+  </si>
+  <si>
+    <t>return mean rolling std 21 trading days</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Last, mean, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rmean 21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, other, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>scale 1.000.000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Last, mean, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, rmean, corr, beta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>scale 1.000.000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Last, mean, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rmean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <t>close return vs vix close return</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mean disp, last dips, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rolling mean 21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inf, mv, mean, last, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rmean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mean_number, last_number, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rolling mean 21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mean, last, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rmean 21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>price_q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, da_norm_q, dis_norm_q, mae_norm_q</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -320,7 +677,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +687,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,15 +724,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,15 +1013,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
@@ -655,34 +1029,34 @@
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -694,21 +1068,21 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>1.5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>63</v>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
@@ -720,22 +1094,22 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
+      <c r="E3" s="12">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>65</v>
+      <c r="I3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -746,22 +1120,22 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>1.5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>66</v>
+      <c r="I4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -772,21 +1146,21 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
-        <v>1.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -798,15 +1172,15 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="E6" s="12">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
@@ -818,15 +1192,15 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6" t="s">
+      <c r="E7" s="12">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -838,16 +1212,18 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8">
-        <v>1.5</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6" t="s">
-        <v>69</v>
+      <c r="E8" s="12">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -858,15 +1234,15 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9">
-        <v>1.5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="6" t="s">
+      <c r="E9" s="12">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -878,15 +1254,17 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10">
-        <v>1.5</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="6" t="s">
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
@@ -898,15 +1276,17 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="E11">
-        <v>1.5</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+      <c r="E11" s="12">
+        <v>3</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
@@ -918,13 +1298,18 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>26</v>
+      <c r="E12" s="12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -933,115 +1318,120 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="E14">
-        <v>1.5</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6" t="s">
+      <c r="E14" s="12">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15">
-        <v>1</v>
+      <c r="E15" s="12">
+        <v>3</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
-        <v>1.5</v>
+      <c r="E16" s="12">
+        <v>3</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" s="12">
+        <v>3</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E17">
-        <v>1.5</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="6" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" s="12">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="E18">
-        <v>1.5</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1050,74 +1440,103 @@
         <v>7</v>
       </c>
       <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="12">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="12">
+        <v>3</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E21" s="12">
+        <v>3</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E20">
-        <v>1.5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="12">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21">
-        <v>1.5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22">
-        <v>1.5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>56</v>
-      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1141,35 +1560,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1188,12 +1607,12 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regresion tables - 1
</commit_message>
<xml_diff>
--- a/output/determinants/variables_structure.xlsx
+++ b/output/determinants/variables_structure.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Main\DOCUMENTOS\3. MACHINE LEARNING\PYTHON_PROYECTS\LPC_Finance\output\determinants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107471B2-141A-4BB1-B83E-C2E469327759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0850590-BE3D-4108-BAF0-BFDD1D694710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="540" windowWidth="20325" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="REGVARS" sheetId="3" r:id="rId1"/>
-    <sheet name="FIXED INCOME" sheetId="2" r:id="rId2"/>
+    <sheet name="VARS" sheetId="4" r:id="rId1"/>
+    <sheet name="REGVARS" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="148">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -168,39 +168,6 @@
     <t>OPT_DIS</t>
   </si>
   <si>
-    <t>AA - periodo 1</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>pendiente curva</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>retorno accion</t>
-  </si>
-  <si>
-    <t>US1M=RR</t>
-  </si>
-  <si>
-    <t>US30Y=RR</t>
-  </si>
-  <si>
-    <t>Spread largo-corto</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>QUESTIONS</t>
   </si>
   <si>
@@ -625,18 +592,247 @@
       </rPr>
       <t>, da_norm_q, dis_norm_q, mae_norm_q</t>
     </r>
+  </si>
+  <si>
+    <t>DESCRIBE</t>
+  </si>
+  <si>
+    <t>LT-ST Bond Spread BETA with Asset Return</t>
+  </si>
+  <si>
+    <t>SP500 Index Return BETA with Asset Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean of 21 days Rolling Standard Deviation </t>
+  </si>
+  <si>
+    <t>Mean of 252 days Rolling Standard Deviation</t>
+  </si>
+  <si>
+    <t>Market Capitalization of the Firm</t>
+  </si>
+  <si>
+    <t>Price to book per share ratio</t>
+  </si>
+  <si>
+    <t>Streak histogram mean of the asset</t>
+  </si>
+  <si>
+    <t>Hurst exponent of asset's close price</t>
+  </si>
+  <si>
+    <t>Number of cusum breaks in close price</t>
+  </si>
+  <si>
+    <t>Average directional movement index of asset close price</t>
+  </si>
+  <si>
+    <t>VIX Index BETA with Asset Return</t>
+  </si>
+  <si>
+    <t>Coefficient of variation (Relative STD) of EPS estimation by analysts</t>
+  </si>
+  <si>
+    <t>Number of analyst working on the assets</t>
+  </si>
+  <si>
+    <t>Put-Call Ratio of the Asset's Options Market</t>
+  </si>
+  <si>
+    <t>Bid-Ask Spread of the Asset's trade market</t>
+  </si>
+  <si>
+    <t>Maximum Directional Accuracy of Grid Rolling LPC of the asset</t>
+  </si>
+  <si>
+    <t>Minimum Mean Absolute Percent Error of Grid Rolling LPC of the asset</t>
+  </si>
+  <si>
+    <t>Minimum Error Autocorrelation Discriminant of Grid Rolling LPC of the asset</t>
+  </si>
+  <si>
+    <t>SPREAD_BETA</t>
+  </si>
+  <si>
+    <t>MARKET_BETA</t>
+  </si>
+  <si>
+    <t>R_MSTD_ST</t>
+  </si>
+  <si>
+    <t>R_MSTD_LT</t>
+  </si>
+  <si>
+    <t>MARKETCAP_RMEAN</t>
+  </si>
+  <si>
+    <t>VOLUME_CV</t>
+  </si>
+  <si>
+    <t>Coefficient of variation (Relative STD) of trading volume of the asset</t>
+  </si>
+  <si>
+    <t>PBPERSHARE_RMEAN</t>
+  </si>
+  <si>
+    <t>STREAK_HMEAN</t>
+  </si>
+  <si>
+    <t>ADX30D_TREND_DAYS</t>
+  </si>
+  <si>
+    <t>ANALYST_DISPERSION_RMEAN</t>
+  </si>
+  <si>
+    <t>ANALYST_NUMBER_RMEAN</t>
+  </si>
+  <si>
+    <t>PUTCALLRATIO_RMEAN</t>
+  </si>
+  <si>
+    <t>BIDASK_RMEAN</t>
+  </si>
+  <si>
+    <t>PRICE_CUSUM_BREAKS</t>
+  </si>
+  <si>
+    <t>HURST_RANDWALK_DAYS</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>BOND SPREAD BETA</t>
+  </si>
+  <si>
+    <t>MARKET INDEX BETA</t>
+  </si>
+  <si>
+    <t>SHORT TERM MEAN OF ROLLING STD</t>
+  </si>
+  <si>
+    <t>LONG TERM MEAN OF ROLLING STD</t>
+  </si>
+  <si>
+    <t>MARKET CAP ROLLING MEAN</t>
+  </si>
+  <si>
+    <t>VOLUME COEFFICIENT OF VARIATION</t>
+  </si>
+  <si>
+    <t>PRICE TO BOOK PER SHARE ROLLING MEAN</t>
+  </si>
+  <si>
+    <t>STREAK HISTOGRAM STREAK</t>
+  </si>
+  <si>
+    <t>HURST EXPONENT RANDOM WALK DAYS</t>
+  </si>
+  <si>
+    <t>NUMBER OF CUSUM BREAKS OF PRICE</t>
+  </si>
+  <si>
+    <t>TREND DAYS OF 30 DAYS ADX</t>
+  </si>
+  <si>
+    <t>VIX INDEX BETA</t>
+  </si>
+  <si>
+    <t>ANALYST DISPERSION</t>
+  </si>
+  <si>
+    <t>ANALYST NUMBER</t>
+  </si>
+  <si>
+    <t>PUT CALL RATIO ROLLING MEAN</t>
+  </si>
+  <si>
+    <t>BID ASK SPREAD ROLLING MEAN</t>
+  </si>
+  <si>
+    <t>OPTIMUM DA OF LPC</t>
+  </si>
+  <si>
+    <t>OPTIMUM MAPE OF LPC</t>
+  </si>
+  <si>
+    <t>OPTIMUM DIS OF LPC</t>
+  </si>
+  <si>
+    <t>[Market Fundamentals]</t>
+  </si>
+  <si>
+    <t>[Risk Measure]</t>
+  </si>
+  <si>
+    <t>[Firm Characteristics]</t>
+  </si>
+  <si>
+    <t>[Stock Behavior]</t>
+  </si>
+  <si>
+    <t>[Signal Behavior]</t>
+  </si>
+  <si>
+    <t>[Technical Indicator]</t>
+  </si>
+  <si>
+    <t>[Sentiment Indicator]</t>
+  </si>
+  <si>
+    <t>[Modeling Performance]</t>
+  </si>
+  <si>
+    <t>[Fixed Income]</t>
+  </si>
+  <si>
+    <t>[Variable Income]</t>
+  </si>
+  <si>
+    <t>[Volatility]</t>
+  </si>
+  <si>
+    <t>[Company Size]</t>
+  </si>
+  <si>
+    <t>[Growth Oportunities]</t>
+  </si>
+  <si>
+    <t>[Momentum]</t>
+  </si>
+  <si>
+    <t>[Tendency Change]</t>
+  </si>
+  <si>
+    <t>[Attractiveness]</t>
+  </si>
+  <si>
+    <t>[Expectatives]</t>
+  </si>
+  <si>
+    <t>[Liquidity]</t>
+  </si>
+  <si>
+    <t>[Predictibility Metric]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -675,6 +871,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -724,20 +926,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,11 +1215,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC06C0-F0D6-4B90-8733-F9A30B786942}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1046,17 +1673,17 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -1068,21 +1695,21 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="12">
-        <v>3</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>73</v>
+      <c r="E2" s="10">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
@@ -1094,22 +1721,22 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="12">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>74</v>
+      <c r="E3" s="10">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="8" t="s">
-        <v>62</v>
+      <c r="A4" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1120,22 +1747,22 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12">
-        <v>3</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>75</v>
+      <c r="E4" s="10">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="8" t="s">
-        <v>63</v>
+      <c r="A5" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1146,21 +1773,21 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="12">
-        <v>3</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>75</v>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -1172,15 +1799,15 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>61</v>
+      <c r="E6" s="10">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
@@ -1192,15 +1819,15 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12">
-        <v>3</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>61</v>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -1212,18 +1839,18 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="12">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>76</v>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="9" t="s">
-        <v>64</v>
+      <c r="A9" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1234,15 +1861,15 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="12">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>77</v>
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -1254,17 +1881,17 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="12">
-        <v>3</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>78</v>
+      <c r="E10" s="10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="L10" s="4"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
@@ -1276,17 +1903,17 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="12">
-        <v>3</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>65</v>
+      <c r="E11" s="10">
+        <v>3</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="K11" s="4"/>
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
@@ -1298,18 +1925,18 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="12">
-        <v>3</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>69</v>
+      <c r="E12" s="10">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="K12" s="4"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="9" t="s">
-        <v>70</v>
+      <c r="A13" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1320,17 +1947,17 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="12">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>84</v>
+      <c r="E13" s="10">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="K13" s="4"/>
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
@@ -1342,15 +1969,15 @@
       <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="12">
-        <v>3</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>71</v>
+      <c r="E14" s="10">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
@@ -1362,15 +1989,15 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="12">
-        <v>3</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>79</v>
+      <c r="E15" s="10">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B16" t="s">
@@ -1382,15 +2009,15 @@
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="12">
-        <v>3</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>80</v>
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
@@ -1402,15 +2029,15 @@
       <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="12">
-        <v>3</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>82</v>
+      <c r="E17" s="10">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
@@ -1422,15 +2049,15 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="12">
-        <v>3</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>81</v>
+      <c r="E18" s="10">
+        <v>3</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
@@ -1442,16 +2069,16 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="12">
-        <v>3</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>83</v>
+      <c r="E19" s="10">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="9" t="s">
-        <v>66</v>
+      <c r="A20" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>6</v>
@@ -1460,73 +2087,73 @@
         <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="12">
+        <v>56</v>
+      </c>
+      <c r="E20" s="10">
         <v>3</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="12">
-        <v>3</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>72</v>
+      <c r="E21" s="10">
+        <v>3</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="12">
-        <v>3</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>72</v>
+      <c r="E22" s="10">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="12">
-        <v>3</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>72</v>
+      <c r="E23" s="10">
+        <v>3</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1542,80 +2169,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f>D4-C4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>